<commit_message>
added more checks in 'firstOrderCheck'
</commit_message>
<xml_diff>
--- a/resources/firstOrderCheck.xlsx
+++ b/resources/firstOrderCheck.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recherche\projets\Qparser\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\recherche\fuzzyCalculator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3B6764-0105-429B-9F11-D30BEB5EB7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D0F501-640E-4C5F-B06A-D82280B000DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41760" yWindow="1155" windowWidth="25425" windowHeight="18060" xr2:uid="{DB1751ED-BCAF-4A8B-BBB1-B3D9B7C224F1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{DB1751ED-BCAF-4A8B-BBB1-B3D9B7C224F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="19">
   <si>
     <t>a...z</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>1st char</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Syntax error</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,6 +319,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,7 +347,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -648,109 +663,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE24A54-584F-4A19-87BF-19666F4D98CE}">
-  <dimension ref="A5:R22"/>
+  <dimension ref="A2:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="18" width="7.140625" customWidth="1"/>
+    <col min="4" max="18" width="7.1328125" customWidth="1"/>
+    <col min="22" max="22" width="16.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="D6" s="23" t="s">
+    <row r="2" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="2"/>
+      <c r="D3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="25"/>
-    </row>
-    <row r="7" spans="1:18" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="25"/>
+    </row>
+    <row r="4" spans="1:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="6" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="R4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="str">
+        <f>D4</f>
+        <v>a...z</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="4" t="str">
+        <f>E4</f>
+        <v>0...9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="4" t="str">
+        <f>F4</f>
+        <v>.</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="4" t="str">
-        <f>D7</f>
-        <v>a...z</v>
+        <f>G4</f>
+        <v>_</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>14</v>
@@ -797,13 +978,19 @@
       <c r="R8" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U8" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="21"/>
       <c r="C9" s="4" t="str">
-        <f>E7</f>
-        <v>0...9</v>
+        <f>H4</f>
+        <v>,</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>14</v>
@@ -817,13 +1004,13 @@
       <c r="G9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="8" t="s">
@@ -832,31 +1019,31 @@
       <c r="L9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="21"/>
       <c r="C10" s="4" t="str">
-        <f>F7</f>
-        <v>.</v>
+        <f>I4</f>
+        <v>(</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>14</v>
@@ -864,7 +1051,7 @@
       <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -876,7 +1063,7 @@
       <c r="I10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="8" t="s">
@@ -885,31 +1072,31 @@
       <c r="L10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="9" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R10" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="21"/>
       <c r="C11" s="4" t="str">
-        <f>G7</f>
-        <v>_</v>
+        <f>J4</f>
+        <v>)</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>14</v>
@@ -957,12 +1144,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="21"/>
       <c r="C12" s="4" t="str">
-        <f>H7</f>
-        <v>,</v>
+        <f>K4</f>
+        <v>|</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>14</v>
@@ -976,13 +1163,13 @@
       <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="8" t="s">
@@ -991,32 +1178,29 @@
       <c r="L12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="4" t="str">
-        <f>I7</f>
-        <v>(</v>
-      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1035,7 +1219,7 @@
       <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="8" t="s">
@@ -1044,31 +1228,31 @@
       <c r="L13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="21"/>
       <c r="C14" s="4" t="str">
-        <f>J7</f>
-        <v>)</v>
+        <f>M4</f>
+        <v>+</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>14</v>
@@ -1082,13 +1266,13 @@
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="8" t="s">
@@ -1097,31 +1281,31 @@
       <c r="L14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="N14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R14" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="21"/>
       <c r="C15" s="4" t="str">
-        <f>K7</f>
-        <v>|</v>
+        <f>N4</f>
+        <v>-</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>14</v>
@@ -1135,44 +1319,47 @@
       <c r="G15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R15" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="str">
+        <f>O4</f>
+        <v>*</v>
+      </c>
       <c r="D16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1185,46 +1372,46 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="8" t="s">
+      <c r="L16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="N16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R16" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="21"/>
       <c r="C17" s="4" t="str">
-        <f>M7</f>
-        <v>+</v>
+        <f>P4</f>
+        <v>/</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>14</v>
@@ -1250,7 +1437,7 @@
       <c r="K17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="9" t="s">
@@ -1272,12 +1459,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="21"/>
       <c r="C18" s="4" t="str">
-        <f>N7</f>
-        <v>-</v>
+        <f>Q4</f>
+        <v>^</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>14</v>
@@ -1309,7 +1496,7 @@
       <c r="M18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="O18" s="9" t="s">
@@ -1325,222 +1512,63 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="4" t="str">
-        <f>O7</f>
-        <v>*</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R19" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="4" t="str">
-        <f>P7</f>
-        <v>/</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="4" t="str">
-        <f>Q7</f>
-        <v>^</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R21" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="11" t="str">
-        <f>R7</f>
+      <c r="B19" s="22"/>
+      <c r="C19" s="11" t="str">
+        <f>R4</f>
         <v>//</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="R22" s="17" t="s">
+      <c r="D19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="17" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B8:B22"/>
-    <mergeCell ref="D6:R6"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="D3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more unit tests added documentation added function signature
</commit_message>
<xml_diff>
--- a/resources/firstOrderCheck.xlsx
+++ b/resources/firstOrderCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\recherche\fuzzyCalculator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D0F501-640E-4C5F-B06A-D82280B000DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9401D065-B896-48CC-887D-B956217F5136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{DB1751ED-BCAF-4A8B-BBB1-B3D9B7C224F1}"/>
   </bookViews>
@@ -247,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -302,32 +302,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE24A54-584F-4A19-87BF-19666F4D98CE}">
   <dimension ref="A2:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -694,23 +691,23 @@
     </row>
     <row r="3" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C3" s="2"/>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="27"/>
     </row>
     <row r="4" spans="1:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
@@ -761,7 +758,7 @@
     </row>
     <row r="5" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="4" t="str">
@@ -816,7 +813,7 @@
     </row>
     <row r="6" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="4" t="str">
         <f>E4</f>
         <v>0...9</v>
@@ -869,7 +866,7 @@
     </row>
     <row r="7" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
-      <c r="B7" s="21"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="4" t="str">
         <f>F4</f>
         <v>.</v>
@@ -922,13 +919,13 @@
       <c r="U7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="28" t="s">
+      <c r="V7" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
-      <c r="B8" s="21"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="4" t="str">
         <f>G4</f>
         <v>_</v>
@@ -978,16 +975,16 @@
       <c r="R8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="V8" s="27" t="s">
+      <c r="U8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
-      <c r="B9" s="21"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="4" t="str">
         <f>H4</f>
         <v>,</v>
@@ -1019,7 +1016,7 @@
       <c r="L9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="N9" s="8" t="s">
@@ -1040,7 +1037,7 @@
     </row>
     <row r="10" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="21"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="4" t="str">
         <f>I4</f>
         <v>(</v>
@@ -1072,7 +1069,7 @@
       <c r="L10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="8" t="s">
@@ -1093,7 +1090,7 @@
     </row>
     <row r="11" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="21"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="4" t="str">
         <f>J4</f>
         <v>)</v>
@@ -1146,7 +1143,7 @@
     </row>
     <row r="12" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="21"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="4" t="str">
         <f>K4</f>
         <v>|</v>
@@ -1199,7 +1196,7 @@
     </row>
     <row r="13" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="21"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
         <v>14</v>
@@ -1249,7 +1246,7 @@
     </row>
     <row r="14" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="21"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="4" t="str">
         <f>M4</f>
         <v>+</v>
@@ -1266,7 +1263,7 @@
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="19" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -1302,7 +1299,7 @@
     </row>
     <row r="15" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
-      <c r="B15" s="21"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="4" t="str">
         <f>N4</f>
         <v>-</v>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="16" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
-      <c r="B16" s="21"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="4" t="str">
         <f>O4</f>
         <v>*</v>
@@ -1408,7 +1405,7 @@
     </row>
     <row r="17" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
-      <c r="B17" s="21"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="4" t="str">
         <f>P4</f>
         <v>/</v>
@@ -1461,7 +1458,7 @@
     </row>
     <row r="18" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="21"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="4" t="str">
         <f>Q4</f>
         <v>^</v>
@@ -1514,7 +1511,7 @@
     </row>
     <row r="19" spans="1:18" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="22"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="11" t="str">
         <f>R4</f>
         <v>//</v>

</xml_diff>